<commit_message>
ka cs pie 67 trent 2-7
</commit_message>
<xml_diff>
--- a/rill-analysis/rill-analysis-report/src/test/resources/ka-cs-pie-6.xlsx
+++ b/rill-analysis/rill-analysis-report/src/test/resources/ka-cs-pie-6.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>url</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -189,6 +189,10 @@
   </si>
   <si>
     <t xml:space="preserve">  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>posId</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -775,8 +779,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="paramTable" displayName="paramTable" ref="A8:G15" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
-  <autoFilter ref="A8:G15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="paramTable" displayName="paramTable" ref="A8:G16" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="A8:G16"/>
   <tableColumns count="7">
     <tableColumn id="1" name="参数" dataDxfId="6"/>
     <tableColumn id="2" name="名称" dataDxfId="5"/>
@@ -1157,7 +1161,7 @@
   <sheetPr codeName="Sheet2">
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1236,73 +1240,73 @@
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="1" t="s">
-        <v>22</v>
+      <c r="A9" s="24" t="s">
+        <v>35</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
         <v>23</v>
       </c>
       <c r="E9" s="12"/>
-      <c r="F9" s="11"/>
+      <c r="F9" s="18"/>
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B11" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="4"/>
+      <c r="C11" s="19"/>
       <c r="D11" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="22"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="12"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="7"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="22"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="23"/>
+        <v>32</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="4"/>
       <c r="D13" s="19" t="s">
         <v>23</v>
       </c>
@@ -1311,13 +1315,13 @@
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="1"/>
+      <c r="A14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="23"/>
       <c r="D14" s="19" t="s">
         <v>23</v>
       </c>
@@ -1326,18 +1330,33 @@
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="25"/>
-      <c r="B15" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="19" t="str">
-        <f>"CS饼图_"</f>
-        <v>CS饼图_</v>
-      </c>
-      <c r="D15" s="19"/>
+      <c r="A15" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="E15" s="12"/>
       <c r="F15" s="18"/>
       <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="25"/>
+      <c r="B16" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="19" t="str">
+        <f>"CS饼图_"</f>
+        <v>CS饼图_</v>
+      </c>
+      <c r="D16" s="19"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>